<commit_message>
ui tweaks, junit testing
</commit_message>
<xml_diff>
--- a/CaseStudyRequirements.xlsx
+++ b/CaseStudyRequirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cena-\Documents\Projects\LocoManage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CFBA10-E955-4F71-B128-38C577E1F56A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA2650B-6731-458E-9E84-3AD914FC2301}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4455" windowWidth="29040" windowHeight="15840" xr2:uid="{7308F507-29E8-4C4B-BB53-BE085C574359}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>All deliverables completed</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -287,19 +290,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -311,32 +301,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -480,23 +450,55 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -509,113 +511,109 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,16 +928,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABAA367-E76E-4A2A-B3F5-4F3367911DD5}">
-  <dimension ref="B1:E66"/>
+  <dimension ref="B1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" customWidth="1"/>
     <col min="4" max="4" width="3" customWidth="1"/>
     <col min="5" max="5" width="72.85546875" customWidth="1"/>
@@ -947,606 +945,608 @@
   <sheetData>
     <row r="1" spans="2:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="30" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="30" t="s">
+      <c r="B12" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="37"/>
+      <c r="C14" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="31"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="37"/>
+      <c r="C16" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="30" t="s">
+      <c r="B17" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="30" t="s">
+      <c r="B18" s="36"/>
+      <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="C19" s="30" t="s">
+      <c r="B19" s="37"/>
+      <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="30" t="s">
+      <c r="B20" s="37"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="31"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="30" t="s">
+      <c r="B21" s="37"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="31"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="30" t="s">
+      <c r="B22" s="37"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="30" t="s">
+      <c r="B24" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="31"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="30" t="s">
+      <c r="B25" s="37"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="31"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="30" t="s">
+      <c r="B26" s="37"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="31"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="32" t="s">
+      <c r="B27" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="24" t="s">
+      <c r="B30" s="37"/>
+      <c r="C30" s="29" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="26"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="39" t="s">
+      <c r="B31" s="42"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="40"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="41" t="s">
+      <c r="B32" s="42"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="42"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="C33" s="27" t="s">
+      <c r="B33" s="37"/>
+      <c r="C33" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="29"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="C34" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="39" t="s">
+      <c r="B34" s="37"/>
+      <c r="C34" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="40"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="11"/>
-      <c r="C35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="30" t="s">
+      <c r="B35" s="37"/>
+      <c r="C35" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="31"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="37"/>
+      <c r="C36" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
-      <c r="C37" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="30" t="s">
+      <c r="B37" s="37"/>
+      <c r="C37" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="31"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="11"/>
-      <c r="C38" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="30" t="s">
+      <c r="B38" s="37"/>
+      <c r="C38" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
-      <c r="C39" s="5" t="s">
+      <c r="B39" s="37"/>
+      <c r="C39" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="41" t="s">
+      <c r="D39" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="42"/>
+      <c r="E39" s="11"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
-      <c r="C40" s="27" t="s">
+      <c r="B40" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="29"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="15"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="39" t="s">
+      <c r="B41" s="37"/>
+      <c r="C41" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="40"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
-      <c r="C42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="41" t="s">
+      <c r="B42" s="37"/>
+      <c r="C42" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="42"/>
+      <c r="E42" s="11"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="27" t="s">
+      <c r="B43" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="15"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
-      <c r="C44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="43" t="s">
+      <c r="B44" s="37"/>
+      <c r="C44" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="44"/>
+      <c r="E44" s="13"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
-      <c r="C45" s="27" t="s">
+      <c r="B45" s="37"/>
+      <c r="C45" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="28"/>
-      <c r="E45" s="29"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="39" t="s">
+      <c r="B46" s="37"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E46" s="40"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="1"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="33"/>
       <c r="E47" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="11"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="1"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="33"/>
       <c r="E48" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="11"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="30" t="s">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="37"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="31"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="11"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="1"/>
+      <c r="E49" s="5"/>
+      <c r="K49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="37"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="33"/>
       <c r="E50" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="11"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="1"/>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="37"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E51" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="11"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="1"/>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="37"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="33"/>
       <c r="E52" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="11"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="1"/>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="37"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E53" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="14"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="4" t="s">
+    <row r="54" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="39"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="15" t="s">
+    <row r="55" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="17"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="39" t="s">
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="18"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D57" s="39"/>
-      <c r="E57" s="40"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="30" t="s">
+      <c r="D57" s="8"/>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D58" s="30"/>
-      <c r="E58" s="31"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="7"/>
-      <c r="C59" s="30" t="s">
+      <c r="D58" s="4"/>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="36"/>
+      <c r="C59" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="30"/>
-      <c r="E59" s="31"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="30" t="s">
+      <c r="D59" s="4"/>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D60" s="30"/>
-      <c r="E60" s="31"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="11"/>
-      <c r="C61" s="1" t="s">
+      <c r="D60" s="4"/>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="37"/>
+      <c r="C61" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E61" s="31"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="11"/>
-      <c r="C62" s="1" t="s">
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="37"/>
+      <c r="C62" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="30" t="s">
+      <c r="D62" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E62" s="31"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="11"/>
-      <c r="C63" s="1" t="s">
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="37"/>
+      <c r="C63" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="30" t="s">
+      <c r="D63" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E63" s="31"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="7"/>
-      <c r="C64" s="30" t="s">
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D64" s="30"/>
-      <c r="E64" s="31"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="5"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" s="30" t="s">
+      <c r="B65" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D65" s="30"/>
-      <c r="E65" s="31"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="5"/>
     </row>
     <row r="66" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="32" t="s">
+      <c r="B66" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D66" s="32"/>
-      <c r="E66" s="33"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D10:E10"/>
+  <mergeCells count="69">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B45:B54"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B29:E29"/>
@@ -1563,22 +1563,41 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B45:B54"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="C49:C54"/>
-    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
layout view works! color changes
</commit_message>
<xml_diff>
--- a/CaseStudyRequirements.xlsx
+++ b/CaseStudyRequirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cena-\Documents\Projects\LocoManage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C179BC31-8F8A-4FB0-BBCD-9DADA3E88E84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2783A23C-CBBE-471A-8770-D8183EA51097}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7308F507-29E8-4C4B-BB53-BE085C574359}"/>
+    <workbookView xWindow="2610" yWindow="0" windowWidth="20250" windowHeight="11385" xr2:uid="{7308F507-29E8-4C4B-BB53-BE085C574359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,75 +545,75 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,7 +931,7 @@
   <dimension ref="B1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:E19"/>
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,108 +948,108 @@
       <c r="B2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="4" t="s">
         <v>63</v>
       </c>
@@ -1059,232 +1059,232 @@
       <c r="E13" s="38"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="39"/>
+      <c r="C19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="16"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="29" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
-      <c r="E23" s="28"/>
+      <c r="E23" s="30"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="14" t="s">
+      <c r="B24" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="16"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="15"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="16"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="15"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="36"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="16"/>
-      <c r="C30" s="32" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="17"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="13"/>
+      <c r="E31" s="17"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="17"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="40"/>
+      <c r="E32" s="19"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="16"/>
-      <c r="C33" s="33" t="s">
+      <c r="B33" s="39"/>
+      <c r="C33" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="23"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="16"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="13"/>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="16"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="15"/>
+      <c r="E35" s="13"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="16"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="15"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="16"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="15"/>
+      <c r="E37" s="13"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="16"/>
+      <c r="B38" s="39"/>
       <c r="C38" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="15"/>
+      <c r="E38" s="13"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="16"/>
+      <c r="B39" s="39"/>
       <c r="C39" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D39" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="40"/>
+      <c r="E39" s="19"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="39" t="s">
         <v>65</v>
       </c>
       <c r="C40" s="22" t="s">
@@ -1294,27 +1294,27 @@
       <c r="E40" s="23"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="16"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="13"/>
+      <c r="E41" s="17"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="16"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="40"/>
+      <c r="E42" s="19"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="39" t="s">
         <v>65</v>
       </c>
       <c r="C43" s="22" t="s">
@@ -1324,17 +1324,17 @@
       <c r="E43" s="23"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="16"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="41" t="s">
+      <c r="D44" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="42"/>
+      <c r="E44" s="21"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="16"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="22" t="s">
         <v>40</v>
       </c>
@@ -1342,15 +1342,15 @@
       <c r="E45" s="23"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="16"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="24"/>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E46" s="13"/>
+      <c r="E46" s="17"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="16"/>
+      <c r="B47" s="39"/>
       <c r="C47" s="24"/>
       <c r="D47" s="7"/>
       <c r="E47" s="2" t="s">
@@ -1358,7 +1358,7 @@
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="16"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="24"/>
       <c r="D48" s="7"/>
       <c r="E48" s="2" t="s">
@@ -1366,18 +1366,18 @@
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="16"/>
+      <c r="B49" s="39"/>
       <c r="C49" s="24"/>
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="15"/>
+      <c r="E49" s="13"/>
       <c r="K49" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="16"/>
+      <c r="B50" s="39"/>
       <c r="C50" s="24"/>
       <c r="D50" s="7"/>
       <c r="E50" s="2" t="s">
@@ -1385,7 +1385,7 @@
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="16"/>
+      <c r="B51" s="39"/>
       <c r="C51" s="24"/>
       <c r="D51" s="7" t="s">
         <v>65</v>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="16"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="24"/>
       <c r="D52" s="7"/>
       <c r="E52" s="2" t="s">
@@ -1403,7 +1403,7 @@
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="16"/>
+      <c r="B53" s="39"/>
       <c r="C53" s="24"/>
       <c r="D53" s="7" t="s">
         <v>65</v>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="54" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="18"/>
+      <c r="B54" s="41"/>
       <c r="C54" s="25"/>
       <c r="D54" s="11"/>
       <c r="E54" s="3" t="s">
@@ -1422,151 +1422,128 @@
     </row>
     <row r="55" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="19" t="s">
+      <c r="B56" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="21"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="28"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="13"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D58" s="14"/>
-      <c r="E58" s="15"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="9"/>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="14"/>
-      <c r="E59" s="15"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="13"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="14" t="s">
+      <c r="B60" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D60" s="14"/>
-      <c r="E60" s="15"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="13"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="16"/>
+      <c r="B61" s="39"/>
       <c r="C61" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E61" s="15"/>
+      <c r="E61" s="13"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="16"/>
+      <c r="B62" s="39"/>
       <c r="C62" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E62" s="15"/>
+      <c r="E62" s="13"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="16"/>
+      <c r="B63" s="39"/>
       <c r="C63" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E63" s="15"/>
+      <c r="E63" s="13"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D64" s="14"/>
-      <c r="E64" s="15"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="13"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D65" s="14"/>
-      <c r="E65" s="15"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="13"/>
     </row>
     <row r="66" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D66" s="35"/>
-      <c r="E66" s="36"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B45:B54"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C46:C48"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B23:E23"/>
@@ -1583,21 +1560,44 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B45:B54"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
comments, user stories, technical challenges
</commit_message>
<xml_diff>
--- a/CaseStudyRequirements.xlsx
+++ b/CaseStudyRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cena-\Documents\Projects\LocoManage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2783A23C-CBBE-471A-8770-D8183EA51097}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30164224-E729-40DE-B08C-139553607654}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2610" yWindow="0" windowWidth="20250" windowHeight="11385" xr2:uid="{7308F507-29E8-4C4B-BB53-BE085C574359}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>All deliverables completed</t>
   </si>
@@ -547,71 +547,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABAA367-E76E-4A2A-B3F5-4F3367911DD5}">
   <dimension ref="B1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,23 +945,23 @@
   <sheetData>
     <row r="1" spans="2:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -971,7 +971,7 @@
       <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
         <v>63</v>
       </c>
@@ -1009,7 +1009,7 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -1019,7 +1019,7 @@
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
@@ -1029,7 +1029,7 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="4" t="s">
         <v>63</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -1049,17 +1049,17 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="35"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="4" t="s">
         <v>63</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1079,7 +1079,7 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="5" t="s">
         <v>63</v>
       </c>
@@ -1107,7 +1107,9 @@
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
+      <c r="B19" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="C19" s="12" t="s">
         <v>16</v>
       </c>
@@ -1115,39 +1117,45 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="D20" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="D21" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="39"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="D22" s="12" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="30"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -1157,7 +1165,7 @@
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="6"/>
       <c r="D25" s="12" t="s">
         <v>22</v>
@@ -1165,7 +1173,7 @@
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="39"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="6"/>
       <c r="D26" s="12" t="s">
         <v>21</v>
@@ -1176,65 +1184,65 @@
       <c r="B27" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="33"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="39"/>
-      <c r="C30" s="34" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="36"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="17"/>
+      <c r="E31" s="37"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="40"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="19"/>
+      <c r="E32" s="39"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="39"/>
-      <c r="C33" s="35" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="23"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="39"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="37"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="39"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="7" t="s">
         <v>65</v>
       </c>
@@ -1244,7 +1252,7 @@
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="39"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="7" t="s">
         <v>64</v>
       </c>
@@ -1254,7 +1262,7 @@
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="39"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="7" t="s">
         <v>65</v>
       </c>
@@ -1264,7 +1272,7 @@
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="39"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="7" t="s">
         <v>65</v>
       </c>
@@ -1274,100 +1282,100 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="39"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="19"/>
+      <c r="E39" s="39"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="22" t="s">
+      <c r="B40" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="23"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="21"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="39"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="17"/>
+      <c r="E41" s="37"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="39"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="19"/>
+      <c r="E42" s="39"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="22" t="s">
+      <c r="B43" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="23"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="39"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="21"/>
+      <c r="E44" s="41"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="39"/>
-      <c r="C45" s="22" t="s">
+      <c r="B45" s="14"/>
+      <c r="C45" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="23"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="39"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="16" t="s">
+      <c r="B46" s="14"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E46" s="17"/>
+      <c r="E46" s="37"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="39"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="22"/>
       <c r="D47" s="7"/>
       <c r="E47" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="39"/>
-      <c r="C48" s="24"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="22"/>
       <c r="D48" s="7"/>
       <c r="E48" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="39"/>
-      <c r="C49" s="24"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="12" t="s">
         <v>44</v>
       </c>
@@ -1377,16 +1385,16 @@
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="39"/>
-      <c r="C50" s="24"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="22"/>
       <c r="D50" s="7"/>
       <c r="E50" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="39"/>
-      <c r="C51" s="24"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="7" t="s">
         <v>65</v>
       </c>
@@ -1395,16 +1403,16 @@
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="39"/>
-      <c r="C52" s="24"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="22"/>
       <c r="D52" s="7"/>
       <c r="E52" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="39"/>
-      <c r="C53" s="24"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="22"/>
       <c r="D53" s="7" t="s">
         <v>65</v>
       </c>
@@ -1413,8 +1421,8 @@
       </c>
     </row>
     <row r="54" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="41"/>
-      <c r="C54" s="25"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="42"/>
       <c r="D54" s="11"/>
       <c r="E54" s="3" t="s">
         <v>49</v>
@@ -1422,22 +1430,22 @@
     </row>
     <row r="55" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="28"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="19"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="17"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="37"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
@@ -1458,7 +1466,7 @@
       <c r="E59" s="13"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="39" t="s">
+      <c r="B60" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C60" s="12" t="s">
@@ -1468,7 +1476,7 @@
       <c r="E60" s="13"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="39"/>
+      <c r="B61" s="14"/>
       <c r="C61" s="7" t="s">
         <v>63</v>
       </c>
@@ -1478,7 +1486,7 @@
       <c r="E61" s="13"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="39"/>
+      <c r="B62" s="14"/>
       <c r="C62" s="7" t="s">
         <v>63</v>
       </c>
@@ -1488,7 +1496,7 @@
       <c r="E62" s="13"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="39"/>
+      <c r="B63" s="14"/>
       <c r="C63" s="7" t="s">
         <v>63</v>
       </c>
@@ -1521,14 +1529,67 @@
       <c r="B66" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D66" s="14"/>
-      <c r="E66" s="15"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C6:E6"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="B60:B63"/>
     <mergeCell ref="B4:B5"/>
@@ -1545,59 +1606,6 @@
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="C46:C48"/>
     <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C49:C54"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>